<commit_message>
Lea converted xlsx to csv
</commit_message>
<xml_diff>
--- a/data/Vegetationsaufnahmen_Rohdaten.xlsx
+++ b/data/Vegetationsaufnahmen_Rohdaten.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1757963_ed_ac_uk/Documents/bachelor/data collection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lea\Documents\R\git\bachelor_diss\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7804BBE4-1748-42E2-B579-5C3E86AB77CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0F9002-84C3-4CBF-B740-B19F0D26CB3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" tabRatio="811" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="344">
   <si>
     <t>Achillea millefolium</t>
   </si>
@@ -768,18 +768,9 @@
     <t>Veronica scutellata</t>
   </si>
   <si>
-    <t>11A1</t>
-  </si>
-  <si>
-    <t>11B1</t>
-  </si>
-  <si>
     <t>Viola spec.</t>
   </si>
   <si>
-    <t>11C1</t>
-  </si>
-  <si>
     <t>11D</t>
   </si>
   <si>
@@ -1081,6 +1072,15 @@
   </si>
   <si>
     <t>Calthion bis Niedermoor, ich würde hier noch selektieren auf Calthion (Ordination, Tabellen nach Stetigkeiten sortieren oder einfach Plots mit hoher Abundanz von Nardus raus?)</t>
+  </si>
+  <si>
+    <t>11A</t>
+  </si>
+  <si>
+    <t>11B</t>
+  </si>
+  <si>
+    <t>11C</t>
   </si>
 </sst>
 </file>
@@ -2759,7 +2759,7 @@
         <v>147</v>
       </c>
       <c r="AM1" s="141" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="BY1" s="14"/>
       <c r="BZ1" s="14"/>
@@ -2773,7 +2773,7 @@
         <v>150</v>
       </c>
       <c r="AM2" s="141" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:147" x14ac:dyDescent="0.25">
@@ -2781,15 +2781,15 @@
         <v>219</v>
       </c>
       <c r="AE3" s="117" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="AM3" s="141" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:147" x14ac:dyDescent="0.25">
       <c r="B5" s="38" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="W5" s="5"/>
       <c r="Y5" s="5"/>
@@ -2799,13 +2799,13 @@
       <c r="AI5" s="118"/>
       <c r="AK5" s="118"/>
       <c r="AM5" s="141" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="AO5" s="142" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="AQ5" s="109" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="AS5" s="5"/>
       <c r="AU5" s="5"/>
@@ -2826,22 +2826,22 @@
       <c r="BY5" s="5"/>
       <c r="BZ5" s="5"/>
       <c r="CA5" s="167" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="CC5" s="167" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="CD5" s="167"/>
       <c r="CE5" s="167" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="CF5" s="167"/>
       <c r="CG5" s="167" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="CH5" s="167"/>
       <c r="CI5" s="167" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="CJ5" s="167"/>
       <c r="CK5" s="5"/>
@@ -2853,175 +2853,175 @@
         <v>68</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="21" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="12" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="21" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="J6" s="13"/>
       <c r="K6" s="12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="L6" s="12"/>
       <c r="M6" s="21" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="N6" s="13"/>
       <c r="O6" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="P6" s="12"/>
       <c r="Q6" s="21" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="R6" s="13"/>
       <c r="S6" s="12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="T6" s="12"/>
       <c r="U6" s="21" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="V6" s="74"/>
       <c r="W6" s="14" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="X6" s="14"/>
       <c r="Y6" s="23" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="Z6" s="74"/>
       <c r="AA6" s="14" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="AB6" s="14"/>
       <c r="AC6" s="23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="AD6" s="74"/>
       <c r="AE6" s="119" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="AF6" s="119"/>
       <c r="AG6" s="120" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="AH6" s="121"/>
       <c r="AI6" s="119" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="AJ6" s="119"/>
       <c r="AK6" s="120" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="AL6" s="121"/>
       <c r="AM6" s="143" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="AN6" s="143"/>
       <c r="AO6" s="144" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="AP6" s="145"/>
       <c r="AQ6" s="110" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="AR6" s="110"/>
       <c r="AS6" s="23" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="AT6" s="74"/>
       <c r="AU6" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="AV6" s="14"/>
       <c r="AW6" s="23" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="AX6" s="74"/>
       <c r="AY6" s="14" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="AZ6" s="14"/>
       <c r="BA6" s="23" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="BB6" s="74"/>
       <c r="BC6" s="14" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="BD6" s="14"/>
       <c r="BE6" s="23" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="BF6" s="74"/>
       <c r="BG6" s="14" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="BH6" s="14"/>
       <c r="BI6" s="23" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="BJ6" s="74"/>
       <c r="BK6" s="14" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="BL6" s="14"/>
       <c r="BM6" s="23" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="BN6" s="74"/>
       <c r="BO6" s="14" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="BP6" s="14"/>
       <c r="BQ6" s="23" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="BR6" s="74"/>
       <c r="BS6" s="14" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="BT6" s="14"/>
       <c r="BU6" s="23" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="BV6" s="74"/>
       <c r="BW6" s="14" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="BX6" s="14"/>
       <c r="BY6" s="23" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="BZ6" s="74"/>
       <c r="CA6" s="166" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="CB6" s="168"/>
       <c r="CC6" s="166" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="CD6" s="166"/>
       <c r="CE6" s="169" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="CF6" s="166"/>
       <c r="CG6" s="169" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="CH6" s="168"/>
       <c r="CI6" s="166" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="CJ6" s="168"/>
       <c r="CK6" s="14"/>
@@ -3404,190 +3404,190 @@
         <v>214</v>
       </c>
       <c r="C10" s="80" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E10" s="80" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F10" s="81" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I10" s="80" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="J10" s="81" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="M10" s="80" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="N10" s="81" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="Q10" s="80" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="R10" s="81" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="S10" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="U10" s="80" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="V10" s="81"/>
       <c r="W10" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="X10" s="5"/>
       <c r="Y10" s="80" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="Z10" s="81"/>
       <c r="AA10" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="AB10" s="5"/>
       <c r="AC10" s="80" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="AD10" s="81"/>
       <c r="AE10" s="118" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="AF10" s="118"/>
       <c r="AG10" s="126" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="AH10" s="127"/>
       <c r="AI10" s="118" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="AJ10" s="118"/>
       <c r="AK10" s="126" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="AL10" s="127"/>
       <c r="AM10" s="142" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AN10" s="142"/>
       <c r="AO10" s="150" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="AP10" s="151"/>
       <c r="AQ10" s="109" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="AR10" s="109"/>
       <c r="AS10" s="80" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="AT10" s="81"/>
       <c r="AU10" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="AV10" s="5"/>
       <c r="AW10" s="80" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="AX10" s="81"/>
       <c r="AY10" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="AZ10" s="5"/>
       <c r="BA10" s="80" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="BB10" s="81"/>
       <c r="BC10" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="BD10" s="5"/>
       <c r="BE10" s="80" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="BF10" s="81"/>
       <c r="BG10" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="BH10" s="5"/>
       <c r="BI10" s="80" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="BJ10" s="81"/>
       <c r="BK10" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="BL10" s="5"/>
       <c r="BM10" s="80" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="BN10" s="81"/>
       <c r="BO10" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="BP10" s="5"/>
       <c r="BQ10" s="80" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="BR10" s="81"/>
       <c r="BS10" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="BT10" s="5"/>
       <c r="BU10" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="BV10" s="81"/>
       <c r="BW10" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="BX10" s="5"/>
       <c r="BY10" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="BZ10" s="81"/>
       <c r="CA10" s="167" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="CB10" s="175"/>
       <c r="CC10" s="167" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="CD10" s="167"/>
       <c r="CE10" s="176" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="CF10" s="167"/>
       <c r="CG10" s="176" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="CH10" s="175"/>
       <c r="CI10" s="167" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="CJ10" s="175"/>
       <c r="CK10" s="5"/>
@@ -3814,84 +3814,84 @@
         <v>223</v>
       </c>
       <c r="C12" s="80" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E12" s="80" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F12" s="81" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I12" s="80" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J12" s="81" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="M12" s="80" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="N12" s="81" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="Q12" s="80" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="R12" s="81" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="T12" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="U12" s="80" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="V12" s="81" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="W12" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="Y12" s="80" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="Z12" s="81" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="AA12" s="5"/>
       <c r="AB12" s="5"/>
       <c r="AC12" s="80" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="AD12" s="81" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="AE12" s="118" t="s">
         <v>225</v>
@@ -4144,7 +4144,7 @@
     </row>
     <row r="14" spans="1:147" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="79" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C14" s="22"/>
       <c r="E14" s="22"/>
@@ -4246,7 +4246,7 @@
     </row>
     <row r="15" spans="1:147" x14ac:dyDescent="0.25">
       <c r="B15" s="79" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C15" s="22">
         <v>72</v>
@@ -4382,7 +4382,7 @@
     </row>
     <row r="16" spans="1:147" x14ac:dyDescent="0.25">
       <c r="B16" s="79" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C16" s="22"/>
       <c r="D16" s="2"/>
@@ -4733,7 +4733,7 @@
     </row>
     <row r="19" spans="2:140" x14ac:dyDescent="0.25">
       <c r="B19" s="79" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C19" s="22">
         <v>1</v>
@@ -6150,7 +6150,7 @@
     </row>
     <row r="31" spans="2:140" x14ac:dyDescent="0.25">
       <c r="B31" s="79" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C31" s="22"/>
       <c r="D31" s="2"/>
@@ -6208,7 +6208,7 @@
     </row>
     <row r="32" spans="2:140" x14ac:dyDescent="0.25">
       <c r="B32" s="79" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C32" s="22"/>
       <c r="D32" s="2"/>
@@ -6266,7 +6266,7 @@
     </row>
     <row r="33" spans="1:139" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="79" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C33" s="22"/>
       <c r="E33" s="22"/>
@@ -7073,7 +7073,7 @@
         <v>93</v>
       </c>
       <c r="B40" s="89" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C40" s="22"/>
       <c r="D40" s="2"/>
@@ -7138,7 +7138,7 @@
         <v>93</v>
       </c>
       <c r="B41" s="93" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C41" s="22"/>
       <c r="D41" s="2"/>
@@ -9815,7 +9815,7 @@
         <v>93</v>
       </c>
       <c r="B70" s="89" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C70" s="22"/>
       <c r="D70" s="2"/>
@@ -10528,7 +10528,7 @@
         <v>93</v>
       </c>
       <c r="B78" s="79" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C78" s="22"/>
       <c r="E78" s="22"/>
@@ -10987,7 +10987,7 @@
         <v>92</v>
       </c>
       <c r="B83" s="93" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C83" s="22"/>
       <c r="D83" s="2"/>
@@ -11257,7 +11257,7 @@
         <v>92</v>
       </c>
       <c r="B87" s="96" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C87" s="50"/>
       <c r="D87" s="97"/>
@@ -11534,7 +11534,7 @@
         <v>92</v>
       </c>
       <c r="B91" s="94" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C91" s="22"/>
       <c r="D91" s="2"/>
@@ -12288,7 +12288,7 @@
         <v>92</v>
       </c>
       <c r="B103" s="89" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C103" s="22"/>
       <c r="D103" s="2"/>
@@ -12499,7 +12499,7 @@
         <v>92</v>
       </c>
       <c r="B106" s="90" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C106" s="22"/>
       <c r="D106" s="2"/>
@@ -12560,7 +12560,7 @@
         <v>92</v>
       </c>
       <c r="B107" s="90" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C107" s="22"/>
       <c r="D107" s="2"/>
@@ -12682,7 +12682,7 @@
         <v>92</v>
       </c>
       <c r="B109" s="90" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C109" s="22"/>
       <c r="D109" s="2"/>
@@ -12743,7 +12743,7 @@
         <v>92</v>
       </c>
       <c r="B110" s="90" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C110" s="22"/>
       <c r="D110" s="2"/>
@@ -12940,7 +12940,7 @@
         <v>92</v>
       </c>
       <c r="B113" s="93" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C113" s="22"/>
       <c r="D113" s="2"/>
@@ -13123,7 +13123,7 @@
         <v>92</v>
       </c>
       <c r="B116" s="79" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C116" s="22"/>
       <c r="D116" s="2"/>
@@ -13423,7 +13423,7 @@
         <v>19</v>
       </c>
       <c r="BU119" s="22" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="BV119" s="67"/>
       <c r="BY119" s="22"/>
@@ -13945,7 +13945,7 @@
         <v>92</v>
       </c>
       <c r="B125" s="90" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C125" s="22"/>
       <c r="D125" s="2"/>
@@ -14499,7 +14499,7 @@
         <v>92</v>
       </c>
       <c r="B132" s="92" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C132" s="22"/>
       <c r="D132" s="2"/>
@@ -14627,7 +14627,7 @@
         <v>92</v>
       </c>
       <c r="B134" s="93" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C134" s="22"/>
       <c r="D134" s="2"/>
@@ -15319,7 +15319,7 @@
         <v>92</v>
       </c>
       <c r="B144" s="90" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C144" s="22"/>
       <c r="D144" s="2"/>
@@ -15506,7 +15506,7 @@
         <v>92</v>
       </c>
       <c r="B147" s="89" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C147" s="22"/>
       <c r="D147" s="2"/>
@@ -15692,7 +15692,7 @@
         <v>12</v>
       </c>
       <c r="BU148" s="22" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="BV148" s="67"/>
       <c r="BW148" s="2">
@@ -15961,7 +15961,7 @@
         <v>92</v>
       </c>
       <c r="B152" s="92" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C152" s="22"/>
       <c r="D152" s="2"/>
@@ -16792,7 +16792,7 @@
         <v>92</v>
       </c>
       <c r="B161" s="92" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C161" s="22"/>
       <c r="D161" s="2"/>
@@ -17696,7 +17696,7 @@
       <c r="AK172" s="122"/>
       <c r="AL172" s="123"/>
       <c r="AM172" s="141" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="AO172" s="146"/>
       <c r="AP172" s="147"/>
@@ -17855,7 +17855,7 @@
         <v>92</v>
       </c>
       <c r="B175" s="93" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C175" s="22"/>
       <c r="D175" s="2"/>
@@ -18832,7 +18832,7 @@
         <v>92</v>
       </c>
       <c r="B185" s="93" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C185" s="22"/>
       <c r="D185" s="2"/>
@@ -18934,7 +18934,7 @@
         <v>92</v>
       </c>
       <c r="B186" s="89" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C186" s="22"/>
       <c r="E186" s="22"/>
@@ -19343,7 +19343,7 @@
         <v>94</v>
       </c>
       <c r="B191" s="89" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C191" s="22"/>
       <c r="D191" s="2"/>
@@ -19547,10 +19547,10 @@
     </row>
     <row r="193" spans="1:140" x14ac:dyDescent="0.25">
       <c r="A193" s="101" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B193" s="90" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C193" s="22"/>
       <c r="D193" s="2"/>
@@ -19608,7 +19608,7 @@
     </row>
     <row r="194" spans="1:140" x14ac:dyDescent="0.25">
       <c r="A194" s="101" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B194" s="89" t="s">
         <v>89</v>
@@ -20075,11 +20075,11 @@
   <dimension ref="A1:FA169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="20" workbookViewId="0">
-      <pane xSplit="5790" ySplit="720" topLeftCell="C1" activePane="bottomRight"/>
+      <pane xSplit="5790" ySplit="720" activePane="bottomRight"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight" activeCell="CT1" sqref="CT1:CU1048576"/>
       <selection pane="bottomLeft" activeCell="A62" sqref="A62:XFD62"/>
-      <selection pane="bottomRight" activeCell="CM3" sqref="CM3"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20194,7 +20194,7 @@
   <sheetData>
     <row r="1" spans="1:157" x14ac:dyDescent="0.25">
       <c r="B1" s="38" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F1" s="77"/>
       <c r="I1" s="76"/>
@@ -20210,7 +20210,7 @@
         <v>147</v>
       </c>
       <c r="CM2" s="146" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="CX2" s="193"/>
       <c r="CY2" s="194"/>
@@ -20231,7 +20231,7 @@
         <v>222</v>
       </c>
       <c r="CX3" s="193" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="CY3" s="194"/>
       <c r="CZ3" s="193"/>
@@ -20260,29 +20260,29 @@
     </row>
     <row r="5" spans="1:157" x14ac:dyDescent="0.25">
       <c r="C5" s="223" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="AI5" s="225" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="CX5" s="195" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="CY5" s="194"/>
       <c r="CZ5" s="195" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="DA5" s="194"/>
       <c r="DB5" s="195" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="DC5" s="194"/>
       <c r="DD5" s="195" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="DE5" s="194"/>
       <c r="DF5" s="195" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="DG5" s="194"/>
     </row>
@@ -20646,23 +20646,23 @@
         <v>212</v>
       </c>
       <c r="CX7" s="195" t="s">
-        <v>239</v>
+        <v>341</v>
       </c>
       <c r="CY7" s="196"/>
       <c r="CZ7" s="195" t="s">
-        <v>240</v>
+        <v>342</v>
       </c>
       <c r="DA7" s="196"/>
       <c r="DB7" s="195" t="s">
-        <v>242</v>
+        <v>343</v>
       </c>
       <c r="DC7" s="196"/>
       <c r="DD7" s="195" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="DE7" s="196"/>
       <c r="DF7" s="195" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="DG7" s="194"/>
     </row>
@@ -21725,7 +21725,9 @@
       <c r="B13" s="72" t="s">
         <v>223</v>
       </c>
-      <c r="C13" s="228"/>
+      <c r="C13" s="228" t="s">
+        <v>225</v>
+      </c>
       <c r="D13" s="229"/>
       <c r="E13" s="5" t="s">
         <v>225</v>
@@ -22153,7 +22155,7 @@
     </row>
     <row r="15" spans="1:157" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="60" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C15" s="225"/>
       <c r="D15" s="232"/>
@@ -27654,7 +27656,7 @@
         <v>92</v>
       </c>
       <c r="B76" s="43" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C76" s="240"/>
       <c r="D76" s="241"/>
@@ -31859,7 +31861,7 @@
         <v>92</v>
       </c>
       <c r="B161" s="43" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C161" s="225"/>
       <c r="CX161" s="198"/>

</xml_diff>